<commit_message>
Antonio we will keep your work but this version is better
</commit_message>
<xml_diff>
--- a/data/New-Data.xlsx
+++ b/data/New-Data.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paezha\Desktop\TEMP\my-example\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwa-my.sharepoint.com/personal/00031300_uwa_edu_au/Documents/Elena/my-example/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC919EE-FE73-41F5-BDD1-A4F1440F4A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4BC919EE-FE73-41F5-BDD1-A4F1440F4A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63F68494-EF7B-47AE-A362-3A570AAC616B}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>UID</t>
   </si>
@@ -36,7 +47,10 @@
     <t>Long</t>
   </si>
   <si>
-    <t>"0000001"</t>
+    <t>"0000003"</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
 </sst>
 </file>
@@ -354,15 +368,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -372,8 +386,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>